<commit_message>
Inclusión de archivo wbs_correct con asignación de wbs y ajustes
</commit_message>
<xml_diff>
--- a/data/raw/3616 La Union.xlsx
+++ b/data/raw/3616 La Union.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/14146208daf86e90/9. Valor Ganado/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_8D2CB88AA067BA7A0F7B93D2970ED862135AEC3D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD5E7394-F8B9-491A-A1E4-AB2409C83974}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_8D2CB88AA067BA7A0F7B93D2970ED862135AEC3D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8631EEE2-0AAB-475B-9341-250FABE078AF}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4061,10 +4061,10 @@
   <dimension ref="A1:CB427"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" outlineLevelRow="3" x14ac:dyDescent="0.35"/>
@@ -4770,7 +4770,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="4" spans="1:77" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:77" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>16</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>24</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:77" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:77" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>36</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>38</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>41</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>44</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>47</v>
       </c>
@@ -7100,7 +7100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>50</v>
       </c>
@@ -7320,7 +7320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>53</v>
       </c>
@@ -7540,7 +7540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>55</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>58</v>
       </c>
@@ -7978,7 +7978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>60</v>
       </c>
@@ -8198,7 +8198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>62</v>
       </c>
@@ -8398,7 +8398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>65</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
         <v>67</v>
       </c>
@@ -8776,7 +8776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="s">
         <v>70</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="s">
         <v>73</v>
       </c>
@@ -9160,7 +9160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A25" s="14" t="s">
         <v>76</v>
       </c>
@@ -9284,7 +9284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:77" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:77" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>78</v>
       </c>
@@ -9498,7 +9498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
         <v>82</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
         <v>84</v>
       </c>
@@ -9922,7 +9922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="s">
         <v>86</v>
       </c>
@@ -10088,7 +10088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
         <v>89</v>
       </c>
@@ -10262,7 +10262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>92</v>
       </c>
@@ -10424,7 +10424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
         <v>95</v>
       </c>
@@ -10574,7 +10574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
         <v>98</v>
       </c>
@@ -10716,7 +10716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>101</v>
       </c>
@@ -10856,7 +10856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:80" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>103</v>
       </c>
@@ -11000,7 +11000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
         <v>106</v>
       </c>
@@ -11142,7 +11142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
         <v>108</v>
       </c>
@@ -11282,7 +11282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:80" s="19" customFormat="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:80" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>110</v>
       </c>
@@ -11513,7 +11513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
         <v>112</v>
       </c>
@@ -11744,7 +11744,7 @@
       </c>
       <c r="CB39" s="24"/>
     </row>
-    <row r="40" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
         <v>116</v>
       </c>
@@ -11975,7 +11975,7 @@
       </c>
       <c r="CB40" s="24"/>
     </row>
-    <row r="41" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
         <v>118</v>
       </c>
@@ -12166,7 +12166,7 @@
       </c>
       <c r="CB41" s="24"/>
     </row>
-    <row r="42" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
         <v>122</v>
       </c>
@@ -12357,7 +12357,7 @@
       </c>
       <c r="CB42" s="24"/>
     </row>
-    <row r="43" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
         <v>124</v>
       </c>
@@ -12548,7 +12548,7 @@
       </c>
       <c r="CB43" s="24"/>
     </row>
-    <row r="44" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
         <v>128</v>
       </c>
@@ -12739,7 +12739,7 @@
       </c>
       <c r="CB44" s="24"/>
     </row>
-    <row r="45" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A45" s="15" t="s">
         <v>130</v>
       </c>
@@ -12930,7 +12930,7 @@
       </c>
       <c r="CB45" s="24"/>
     </row>
-    <row r="46" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A46" s="15" t="s">
         <v>132</v>
       </c>
@@ -13121,7 +13121,7 @@
       </c>
       <c r="CB46" s="24"/>
     </row>
-    <row r="47" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
         <v>134</v>
       </c>
@@ -13352,7 +13352,7 @@
       </c>
       <c r="CB47" s="24"/>
     </row>
-    <row r="48" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A48" s="15" t="s">
         <v>136</v>
       </c>
@@ -13583,7 +13583,7 @@
       </c>
       <c r="CB48" s="24"/>
     </row>
-    <row r="49" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A49" s="15" t="s">
         <v>138</v>
       </c>
@@ -13701,7 +13701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:80" s="19" customFormat="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:80" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>140</v>
       </c>
@@ -13932,7 +13932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:80" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>143</v>
       </c>
@@ -14163,7 +14163,7 @@
       </c>
       <c r="CB51" s="24"/>
     </row>
-    <row r="52" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>147</v>
       </c>
@@ -14394,7 +14394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>149</v>
       </c>
@@ -14623,7 +14623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A54" s="15" t="s">
         <v>154</v>
       </c>
@@ -14852,7 +14852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A55" s="15" t="s">
         <v>157</v>
       </c>
@@ -15079,7 +15079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A56" s="15" t="s">
         <v>161</v>
       </c>
@@ -15304,7 +15304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A57" s="15" t="s">
         <v>165</v>
       </c>
@@ -15527,7 +15527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
         <v>169</v>
       </c>
@@ -15756,7 +15756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A59" s="15" t="s">
         <v>172</v>
       </c>
@@ -15985,7 +15985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A60" s="15" t="s">
         <v>174</v>
       </c>
@@ -16212,7 +16212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A61" s="15" t="s">
         <v>176</v>
       </c>
@@ -16437,7 +16437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A62" s="15" t="s">
         <v>178</v>
       </c>
@@ -16660,7 +16660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A63" s="15" t="s">
         <v>183</v>
       </c>
@@ -16871,7 +16871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A64" s="6" t="s">
         <v>185</v>
       </c>
@@ -17102,7 +17102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A65" s="15" t="s">
         <v>189</v>
       </c>
@@ -17333,7 +17333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A66" s="15" t="s">
         <v>192</v>
       </c>
@@ -17562,7 +17562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A67" s="15" t="s">
         <v>194</v>
       </c>
@@ -17787,7 +17787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:80" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
         <v>197</v>
       </c>
@@ -18016,7 +18016,7 @@
       </c>
       <c r="CB68" s="24"/>
     </row>
-    <row r="69" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
         <v>199</v>
       </c>
@@ -18245,7 +18245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A70" s="15" t="s">
         <v>202</v>
       </c>
@@ -18474,7 +18474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="s">
         <v>204</v>
       </c>
@@ -18699,7 +18699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
         <v>206</v>
       </c>
@@ -18924,7 +18924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A73" s="15" t="s">
         <v>209</v>
       </c>
@@ -19127,7 +19127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A74" s="15" t="s">
         <v>214</v>
       </c>
@@ -19330,7 +19330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A75" s="6" t="s">
         <v>216</v>
       </c>
@@ -19519,7 +19519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A76" s="15" t="s">
         <v>219</v>
       </c>
@@ -19708,7 +19708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A77" s="15" t="s">
         <v>221</v>
       </c>
@@ -19881,7 +19881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
         <v>226</v>
       </c>
@@ -20044,7 +20044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A79" s="15" t="s">
         <v>231</v>
       </c>
@@ -20197,7 +20197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A80" s="15" t="s">
         <v>234</v>
       </c>
@@ -20396,7 +20396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A81" s="15" t="s">
         <v>239</v>
       </c>
@@ -20583,7 +20583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A82" s="15" t="s">
         <v>243</v>
       </c>
@@ -20788,7 +20788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A83" s="15" t="s">
         <v>247</v>
       </c>
@@ -20983,7 +20983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
         <v>250</v>
       </c>
@@ -21172,7 +21172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A85" s="15" t="s">
         <v>253</v>
       </c>
@@ -21351,7 +21351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A86" s="15" t="s">
         <v>257</v>
       </c>
@@ -21534,7 +21534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A87" s="15" t="s">
         <v>262</v>
       </c>
@@ -21713,7 +21713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A88" s="15" t="s">
         <v>266</v>
       </c>
@@ -21924,7 +21924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A89" s="15" t="s">
         <v>269</v>
       </c>
@@ -22123,7 +22123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A90" s="6" t="s">
         <v>272</v>
       </c>
@@ -22348,7 +22348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A91" s="15" t="s">
         <v>276</v>
       </c>
@@ -22573,7 +22573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A92" s="15" t="s">
         <v>279</v>
       </c>
@@ -22790,7 +22790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A93" s="15" t="s">
         <v>283</v>
       </c>
@@ -22981,7 +22981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A94" s="15" t="s">
         <v>287</v>
       </c>
@@ -23160,7 +23160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A95" s="15" t="s">
         <v>290</v>
       </c>
@@ -23335,7 +23335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A96" s="15" t="s">
         <v>294</v>
       </c>
@@ -23510,7 +23510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A97" s="15" t="s">
         <v>298</v>
       </c>
@@ -23683,7 +23683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:80" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A98" s="6" t="s">
         <v>300</v>
       </c>
@@ -23882,7 +23882,7 @@
       </c>
       <c r="CB98" s="24"/>
     </row>
-    <row r="99" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A99" s="6" t="s">
         <v>303</v>
       </c>
@@ -24081,7 +24081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A100" s="15" t="s">
         <v>305</v>
       </c>
@@ -24268,7 +24268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A101" s="15" t="s">
         <v>308</v>
       </c>
@@ -24451,7 +24451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A102" s="15" t="s">
         <v>311</v>
       </c>
@@ -24630,7 +24630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A103" s="15" t="s">
         <v>313</v>
       </c>
@@ -24805,7 +24805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A104" s="15" t="s">
         <v>316</v>
       </c>
@@ -24978,7 +24978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A105" s="15" t="s">
         <v>318</v>
       </c>
@@ -25161,7 +25161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A106" s="15" t="s">
         <v>320</v>
       </c>
@@ -25336,7 +25336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A107" s="15" t="s">
         <v>323</v>
       </c>
@@ -25535,7 +25535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A108" s="15" t="s">
         <v>326</v>
       </c>
@@ -25722,7 +25722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A109" s="15" t="s">
         <v>329</v>
       </c>
@@ -25897,7 +25897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A110" s="15" t="s">
         <v>331</v>
       </c>
@@ -26070,7 +26070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
         <v>333</v>
       </c>
@@ -26253,7 +26253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A112" s="15" t="s">
         <v>337</v>
       </c>
@@ -26436,7 +26436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A113" s="15" t="s">
         <v>340</v>
       </c>
@@ -26619,7 +26619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A114" s="15" t="s">
         <v>342</v>
       </c>
@@ -26802,7 +26802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A115" s="15" t="s">
         <v>344</v>
       </c>
@@ -26981,7 +26981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:80" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A116" s="6" t="s">
         <v>347</v>
       </c>
@@ -27212,7 +27212,7 @@
       </c>
       <c r="CB116" s="24"/>
     </row>
-    <row r="117" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A117" s="6" t="s">
         <v>351</v>
       </c>
@@ -27441,7 +27441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A118" s="15" t="s">
         <v>353</v>
       </c>
@@ -27670,7 +27670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A119" s="6" t="s">
         <v>355</v>
       </c>
@@ -27901,7 +27901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A120" s="15" t="s">
         <v>357</v>
       </c>
@@ -28110,7 +28110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A121" s="15" t="s">
         <v>362</v>
       </c>
@@ -28313,7 +28313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A122" s="15" t="s">
         <v>366</v>
       </c>
@@ -28522,7 +28522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A123" s="15" t="s">
         <v>368</v>
       </c>
@@ -28753,7 +28753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A124" s="15" t="s">
         <v>370</v>
       </c>
@@ -28932,7 +28932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A125" s="15" t="s">
         <v>374</v>
       </c>
@@ -29109,7 +29109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A126" s="15" t="s">
         <v>377</v>
       </c>
@@ -29300,7 +29300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A127" s="15" t="s">
         <v>379</v>
       </c>
@@ -29483,7 +29483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A128" s="15" t="s">
         <v>381</v>
       </c>
@@ -29662,7 +29662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A129" s="15" t="s">
         <v>383</v>
       </c>
@@ -29845,7 +29845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A130" s="15" t="s">
         <v>386</v>
       </c>
@@ -30024,7 +30024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A131" s="15" t="s">
         <v>388</v>
       </c>
@@ -30211,7 +30211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A132" s="15" t="s">
         <v>390</v>
       </c>
@@ -30398,7 +30398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A133" s="15" t="s">
         <v>393</v>
       </c>
@@ -30581,7 +30581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A134" s="15" t="s">
         <v>397</v>
       </c>
@@ -30764,7 +30764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:77" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:77" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A135" s="6" t="s">
         <v>400</v>
       </c>
@@ -30972,7 +30972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A136" s="15" t="s">
         <v>404</v>
       </c>
@@ -31181,7 +31181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A137" s="15" t="s">
         <v>407</v>
       </c>
@@ -31386,7 +31386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A138" s="15" t="s">
         <v>410</v>
       </c>
@@ -31591,7 +31591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A139" s="15" t="s">
         <v>413</v>
       </c>
@@ -31790,7 +31790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A140" s="15" t="s">
         <v>417</v>
       </c>
@@ -31987,7 +31987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A141" s="15" t="s">
         <v>421</v>
       </c>
@@ -32182,7 +32182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A142" s="15" t="s">
         <v>424</v>
       </c>
@@ -32373,7 +32373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A143" s="15" t="s">
         <v>427</v>
       </c>
@@ -32560,7 +32560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A144" s="15" t="s">
         <v>431</v>
       </c>
@@ -32747,7 +32747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:80" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A145" s="6" t="s">
         <v>434</v>
       </c>
@@ -32944,7 +32944,7 @@
       </c>
       <c r="CB145" s="24"/>
     </row>
-    <row r="146" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A146" s="15" t="s">
         <v>437</v>
       </c>
@@ -33141,7 +33141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A147" s="15" t="s">
         <v>441</v>
       </c>
@@ -33330,7 +33330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A148" s="15" t="s">
         <v>444</v>
       </c>
@@ -33513,7 +33513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:80" s="19" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:80" s="19" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A149" s="6" t="s">
         <v>446</v>
       </c>
@@ -33701,7 +33701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:80" s="19" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:80" s="19" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A150" s="6" t="s">
         <v>451</v>
       </c>
@@ -33889,7 +33889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:80" s="19" customFormat="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:80" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A151" s="9" t="s">
         <v>453</v>
       </c>
@@ -34112,7 +34112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:80" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A152" s="5" t="s">
         <v>456</v>
       </c>
@@ -34334,7 +34334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A153" s="5" t="s">
         <v>460</v>
       </c>
@@ -34557,7 +34557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A154" s="5" t="s">
         <v>462</v>
       </c>
@@ -34780,7 +34780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A155" s="14" t="s">
         <v>465</v>
       </c>
@@ -35003,7 +35003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A156" s="14" t="s">
         <v>468</v>
       </c>
@@ -35222,7 +35222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A157" s="14" t="s">
         <v>472</v>
       </c>
@@ -35437,7 +35437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A158" s="14" t="s">
         <v>475</v>
       </c>
@@ -35648,7 +35648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A159" s="14" t="s">
         <v>478</v>
       </c>
@@ -35825,7 +35825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A160" s="14" t="s">
         <v>481</v>
       </c>
@@ -36000,7 +36000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A161" s="14" t="s">
         <v>485</v>
       </c>
@@ -36169,7 +36169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
         <v>488</v>
       </c>
@@ -36392,7 +36392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A163" s="14" t="s">
         <v>490</v>
       </c>
@@ -36615,7 +36615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A164" s="14" t="s">
         <v>493</v>
       </c>
@@ -36836,7 +36836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A165" s="14" t="s">
         <v>496</v>
       </c>
@@ -37051,7 +37051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A166" s="14" t="s">
         <v>498</v>
       </c>
@@ -37264,7 +37264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A167" s="14" t="s">
         <v>502</v>
       </c>
@@ -37441,7 +37441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A168" s="14" t="s">
         <v>504</v>
       </c>
@@ -37616,7 +37616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A169" s="14" t="s">
         <v>506</v>
       </c>
@@ -37785,7 +37785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A170" s="5" t="s">
         <v>508</v>
       </c>
@@ -38008,7 +38008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A171" s="14" t="s">
         <v>510</v>
       </c>
@@ -38231,7 +38231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A172" s="14" t="s">
         <v>512</v>
       </c>
@@ -38452,7 +38452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A173" s="14" t="s">
         <v>514</v>
       </c>
@@ -38667,7 +38667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A174" s="14" t="s">
         <v>516</v>
       </c>
@@ -38880,7 +38880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A175" s="14" t="s">
         <v>518</v>
       </c>
@@ -39057,7 +39057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A176" s="14" t="s">
         <v>520</v>
       </c>
@@ -39232,7 +39232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A177" s="14" t="s">
         <v>522</v>
       </c>
@@ -39401,7 +39401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A178" s="5" t="s">
         <v>524</v>
       </c>
@@ -39624,7 +39624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A179" s="14" t="s">
         <v>526</v>
       </c>
@@ -39847,7 +39847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A180" s="14" t="s">
         <v>528</v>
       </c>
@@ -40066,7 +40066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A181" s="14" t="s">
         <v>530</v>
       </c>
@@ -40281,7 +40281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A182" s="14" t="s">
         <v>533</v>
       </c>
@@ -40490,7 +40490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A183" s="14" t="s">
         <v>535</v>
       </c>
@@ -40665,7 +40665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A184" s="14" t="s">
         <v>537</v>
       </c>
@@ -40840,7 +40840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A185" s="14" t="s">
         <v>540</v>
       </c>
@@ -41007,7 +41007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A186" s="5" t="s">
         <v>543</v>
       </c>
@@ -41230,7 +41230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A187" s="14" t="s">
         <v>545</v>
       </c>
@@ -41453,7 +41453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A188" s="14" t="s">
         <v>547</v>
       </c>
@@ -41674,7 +41674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A189" s="14" t="s">
         <v>549</v>
       </c>
@@ -41889,7 +41889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A190" s="14" t="s">
         <v>551</v>
       </c>
@@ -42100,7 +42100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A191" s="14" t="s">
         <v>553</v>
       </c>
@@ -42277,7 +42277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A192" s="14" t="s">
         <v>555</v>
       </c>
@@ -42452,7 +42452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A193" s="14" t="s">
         <v>557</v>
       </c>
@@ -42621,7 +42621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:80" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A194" s="5" t="s">
         <v>559</v>
       </c>
@@ -42803,7 +42803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A195" s="14" t="s">
         <v>563</v>
       </c>
@@ -42986,7 +42986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A196" s="14" t="s">
         <v>565</v>
       </c>
@@ -43165,7 +43165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A197" s="14" t="s">
         <v>567</v>
       </c>
@@ -43342,7 +43342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A198" s="14" t="s">
         <v>570</v>
       </c>
@@ -43519,7 +43519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A199" s="14" t="s">
         <v>574</v>
       </c>
@@ -43684,7 +43684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A200" s="14" t="s">
         <v>578</v>
       </c>
@@ -43847,7 +43847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:80" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A201" s="5" t="s">
         <v>580</v>
       </c>
@@ -44036,7 +44036,7 @@
       </c>
       <c r="CB201" s="24"/>
     </row>
-    <row r="202" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A202" s="5" t="s">
         <v>584</v>
       </c>
@@ -44215,7 +44215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A203" s="14" t="s">
         <v>588</v>
       </c>
@@ -44394,7 +44394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A204" s="14" t="s">
         <v>590</v>
       </c>
@@ -44573,7 +44573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A205" s="14" t="s">
         <v>592</v>
       </c>
@@ -44750,7 +44750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A206" s="14" t="s">
         <v>596</v>
       </c>
@@ -44919,7 +44919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A207" s="14" t="s">
         <v>599</v>
       </c>
@@ -45088,7 +45088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A208" s="14" t="s">
         <v>601</v>
       </c>
@@ -45251,7 +45251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A209" s="5" t="s">
         <v>603</v>
       </c>
@@ -45430,7 +45430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A210" s="14" t="s">
         <v>606</v>
       </c>
@@ -45609,7 +45609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A211" s="14" t="s">
         <v>608</v>
       </c>
@@ -45786,7 +45786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A212" s="14" t="s">
         <v>611</v>
       </c>
@@ -45961,7 +45961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A213" s="14" t="s">
         <v>613</v>
       </c>
@@ -46130,7 +46130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A214" s="14" t="s">
         <v>617</v>
       </c>
@@ -46297,7 +46297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A215" s="14" t="s">
         <v>621</v>
       </c>
@@ -46460,7 +46460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A216" s="5" t="s">
         <v>624</v>
       </c>
@@ -46649,7 +46649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A217" s="14" t="s">
         <v>626</v>
       </c>
@@ -46838,7 +46838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A218" s="14" t="s">
         <v>628</v>
       </c>
@@ -47025,7 +47025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A219" s="14" t="s">
         <v>630</v>
       </c>
@@ -47208,7 +47208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A220" s="14" t="s">
         <v>632</v>
       </c>
@@ -47387,7 +47387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A221" s="14" t="s">
         <v>634</v>
       </c>
@@ -47564,7 +47564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A222" s="14" t="s">
         <v>636</v>
       </c>
@@ -47737,7 +47737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A223" s="14" t="s">
         <v>639</v>
       </c>
@@ -47906,7 +47906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A224" s="5" t="s">
         <v>641</v>
       </c>
@@ -48085,7 +48085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A225" s="14" t="s">
         <v>645</v>
       </c>
@@ -48264,7 +48264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A226" s="14" t="s">
         <v>647</v>
       </c>
@@ -48441,7 +48441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A227" s="14" t="s">
         <v>649</v>
       </c>
@@ -48616,7 +48616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A228" s="14" t="s">
         <v>651</v>
       </c>
@@ -48791,7 +48791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A229" s="14" t="s">
         <v>654</v>
       </c>
@@ -48962,7 +48962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A230" s="14" t="s">
         <v>657</v>
       </c>
@@ -49131,7 +49131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A231" s="14" t="s">
         <v>661</v>
       </c>
@@ -49296,7 +49296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A232" s="5" t="s">
         <v>663</v>
       </c>
@@ -49479,7 +49479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A233" s="14" t="s">
         <v>665</v>
       </c>
@@ -49662,7 +49662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A234" s="14" t="s">
         <v>667</v>
       </c>
@@ -49841,7 +49841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A235" s="14" t="s">
         <v>669</v>
       </c>
@@ -50020,7 +50020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A236" s="14" t="s">
         <v>671</v>
       </c>
@@ -50197,7 +50197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A237" s="14" t="s">
         <v>674</v>
       </c>
@@ -50368,7 +50368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A238" s="14" t="s">
         <v>677</v>
       </c>
@@ -50539,7 +50539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A239" s="14" t="s">
         <v>679</v>
       </c>
@@ -50704,7 +50704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:77" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:77" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A240" s="5" t="s">
         <v>682</v>
       </c>
@@ -50927,7 +50927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A241" s="5" t="s">
         <v>684</v>
       </c>
@@ -51149,7 +51149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A242" s="14" t="s">
         <v>686</v>
       </c>
@@ -51372,7 +51372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A243" s="14" t="s">
         <v>688</v>
       </c>
@@ -51593,7 +51593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A244" s="14" t="s">
         <v>690</v>
       </c>
@@ -51810,7 +51810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A245" s="14" t="s">
         <v>692</v>
       </c>
@@ -52025,7 +52025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A246" s="14" t="s">
         <v>695</v>
       </c>
@@ -52194,7 +52194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A247" s="14" t="s">
         <v>699</v>
       </c>
@@ -52363,7 +52363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A248" s="14" t="s">
         <v>702</v>
       </c>
@@ -52516,7 +52516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A249" s="5" t="s">
         <v>705</v>
       </c>
@@ -52698,7 +52698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A250" s="14" t="s">
         <v>708</v>
       </c>
@@ -52881,7 +52881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A251" s="14" t="s">
         <v>710</v>
       </c>
@@ -53060,7 +53060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A252" s="14" t="s">
         <v>712</v>
       </c>
@@ -53239,7 +53239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A253" s="14" t="s">
         <v>714</v>
       </c>
@@ -53416,7 +53416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A254" s="14" t="s">
         <v>716</v>
       </c>
@@ -53585,7 +53585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A255" s="14" t="s">
         <v>718</v>
       </c>
@@ -53752,7 +53752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A256" s="14" t="s">
         <v>721</v>
       </c>
@@ -53913,7 +53913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:80" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A257" s="5" t="s">
         <v>724</v>
       </c>
@@ -54124,7 +54124,7 @@
       </c>
       <c r="CB257" s="24"/>
     </row>
-    <row r="258" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A258" s="5" t="s">
         <v>727</v>
       </c>
@@ -54335,7 +54335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A259" s="14" t="s">
         <v>729</v>
       </c>
@@ -54546,7 +54546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A260" s="14" t="s">
         <v>732</v>
       </c>
@@ -54753,7 +54753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A261" s="14" t="s">
         <v>736</v>
       </c>
@@ -54958,7 +54958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A262" s="14" t="s">
         <v>739</v>
       </c>
@@ -55127,7 +55127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A263" s="14" t="s">
         <v>741</v>
       </c>
@@ -55290,7 +55290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A264" s="5" t="s">
         <v>744</v>
       </c>
@@ -55487,7 +55487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A265" s="14" t="s">
         <v>747</v>
       </c>
@@ -55684,7 +55684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A266" s="14" t="s">
         <v>750</v>
       </c>
@@ -55879,7 +55879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A267" s="14" t="s">
         <v>752</v>
       </c>
@@ -56070,7 +56070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A268" s="14" t="s">
         <v>755</v>
       </c>
@@ -56243,7 +56243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A269" s="14" t="s">
         <v>757</v>
       </c>
@@ -56412,7 +56412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A270" s="14" t="s">
         <v>759</v>
       </c>
@@ -56778,7 +56778,7 @@
       </c>
       <c r="CB271" s="25"/>
     </row>
-    <row r="272" spans="1:80" s="19" customFormat="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:80" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A272" s="9" t="s">
         <v>766</v>
       </c>
@@ -56969,7 +56969,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="273" spans="1:80" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A273" s="5" t="s">
         <v>770</v>
       </c>
@@ -57159,7 +57159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A274" s="14" t="s">
         <v>771</v>
       </c>
@@ -57349,7 +57349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A275" s="14" t="s">
         <v>773</v>
       </c>
@@ -57537,7 +57537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:80" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A276" s="5" t="s">
         <v>776</v>
       </c>
@@ -57726,7 +57726,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="277" spans="1:80" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A277" s="5" t="s">
         <v>778</v>
       </c>
@@ -57915,7 +57915,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="278" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A278" s="5" t="s">
         <v>780</v>
       </c>
@@ -58104,7 +58104,7 @@
       </c>
       <c r="CB278" s="24"/>
     </row>
-    <row r="279" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A279" s="14" t="s">
         <v>782</v>
       </c>
@@ -58293,7 +58293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A280" s="14" t="s">
         <v>784</v>
       </c>
@@ -58480,7 +58480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A281" s="14" t="s">
         <v>787</v>
       </c>
@@ -58663,7 +58663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A282" s="14" t="s">
         <v>789</v>
       </c>
@@ -58846,7 +58846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A283" s="14" t="s">
         <v>792</v>
       </c>
@@ -58991,7 +58991,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="284" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A284" s="14" t="s">
         <v>795</v>
       </c>
@@ -59149,7 +59149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A285" s="14" t="s">
         <v>799</v>
       </c>
@@ -59323,7 +59323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A286" s="5" t="s">
         <v>802</v>
       </c>
@@ -59493,7 +59493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A287" s="14" t="s">
         <v>805</v>
       </c>
@@ -59664,7 +59664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A288" s="14" t="s">
         <v>809</v>
       </c>
@@ -59831,7 +59831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:77" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A289" s="5" t="s">
         <v>813</v>
       </c>
@@ -60014,7 +60014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A290" s="5" t="s">
         <v>817</v>
       </c>
@@ -60197,7 +60197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A291" s="5" t="s">
         <v>819</v>
       </c>
@@ -60379,7 +60379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A292" s="14" t="s">
         <v>821</v>
       </c>
@@ -60562,7 +60562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A293" s="14" t="s">
         <v>823</v>
       </c>
@@ -60741,7 +60741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A294" s="5" t="s">
         <v>825</v>
       </c>
@@ -60919,7 +60919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A295" s="14" t="s">
         <v>828</v>
       </c>
@@ -61098,7 +61098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A296" s="14" t="s">
         <v>829</v>
       </c>
@@ -61277,7 +61277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A297" s="5" t="s">
         <v>831</v>
       </c>
@@ -61437,7 +61437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A298" s="14" t="s">
         <v>833</v>
       </c>
@@ -61598,7 +61598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A299" s="14" t="s">
         <v>835</v>
       </c>
@@ -61757,7 +61757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A300" s="5" t="s">
         <v>837</v>
       </c>
@@ -61935,7 +61935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A301" s="14" t="s">
         <v>839</v>
       </c>
@@ -62114,7 +62114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A302" s="14" t="s">
         <v>840</v>
       </c>
@@ -62291,7 +62291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A303" s="5" t="s">
         <v>841</v>
       </c>
@@ -62467,7 +62467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A304" s="14" t="s">
         <v>844</v>
       </c>
@@ -62644,7 +62644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A305" s="14" t="s">
         <v>845</v>
       </c>
@@ -62819,7 +62819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A306" s="5" t="s">
         <v>846</v>
       </c>
@@ -62993,7 +62993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A307" s="14" t="s">
         <v>850</v>
       </c>
@@ -63167,7 +63167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A308" s="14" t="s">
         <v>851</v>
       </c>
@@ -63339,7 +63339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A309" s="5" t="s">
         <v>853</v>
       </c>
@@ -63517,7 +63517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A310" s="5" t="s">
         <v>855</v>
       </c>
@@ -63699,7 +63699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A311" s="5" t="s">
         <v>858</v>
       </c>
@@ -63861,7 +63861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A312" s="14" t="s">
         <v>860</v>
       </c>
@@ -64024,7 +64024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A313" s="14" t="s">
         <v>863</v>
       </c>
@@ -64185,7 +64185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:77" s="19" customFormat="1" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:77" s="19" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A314" s="5" t="s">
         <v>866</v>
       </c>
@@ -64364,7 +64364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A315" s="14" t="s">
         <v>869</v>
       </c>
@@ -64536,7 +64536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:77" s="19" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:77" s="19" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A316" s="5" t="s">
         <v>873</v>
       </c>
@@ -64715,7 +64715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A317" s="14" t="s">
         <v>875</v>
       </c>
@@ -64893,7 +64893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A318" s="14" t="s">
         <v>879</v>
       </c>
@@ -65059,7 +65059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A319" s="14" t="s">
         <v>882</v>
       </c>
@@ -65229,7 +65229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:77" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A320" s="5" t="s">
         <v>884</v>
       </c>
@@ -65407,7 +65407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A321" s="5" t="s">
         <v>887</v>
       </c>
@@ -65586,7 +65586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A322" s="5" t="s">
         <v>890</v>
       </c>
@@ -65765,7 +65765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A323" s="5" t="s">
         <v>892</v>
       </c>
@@ -65942,7 +65942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A324" s="14" t="s">
         <v>895</v>
       </c>
@@ -66119,7 +66119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A325" s="14" t="s">
         <v>898</v>
       </c>
@@ -66296,7 +66296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A326" s="14" t="s">
         <v>902</v>
       </c>
@@ -66473,7 +66473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A327" s="14" t="s">
         <v>906</v>
       </c>
@@ -66648,7 +66648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A328" s="14" t="s">
         <v>908</v>
       </c>
@@ -66821,7 +66821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A329" s="14" t="s">
         <v>911</v>
       </c>
@@ -66994,7 +66994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A330" s="14" t="s">
         <v>915</v>
       </c>
@@ -67167,7 +67167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A331" s="14" t="s">
         <v>917</v>
       </c>
@@ -67338,7 +67338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A332" s="14" t="s">
         <v>920</v>
       </c>
@@ -67509,7 +67509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A333" s="14" t="s">
         <v>922</v>
       </c>
@@ -67678,7 +67678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A334" s="5" t="s">
         <v>925</v>
       </c>
@@ -67849,7 +67849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A335" s="5" t="s">
         <v>927</v>
       </c>
@@ -68018,7 +68018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A336" s="14" t="s">
         <v>929</v>
       </c>
@@ -68187,7 +68187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A337" s="14" t="s">
         <v>931</v>
       </c>
@@ -68356,7 +68356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A338" s="14" t="s">
         <v>933</v>
       </c>
@@ -68525,7 +68525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A339" s="5" t="s">
         <v>935</v>
       </c>
@@ -68696,7 +68696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A340" s="14" t="s">
         <v>937</v>
       </c>
@@ -68867,7 +68867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A341" s="14" t="s">
         <v>940</v>
       </c>
@@ -69036,7 +69036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A342" s="5" t="s">
         <v>942</v>
       </c>
@@ -69205,7 +69205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A343" s="14" t="s">
         <v>945</v>
       </c>
@@ -69374,7 +69374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A344" s="14" t="s">
         <v>948</v>
       </c>
@@ -69541,7 +69541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A345" s="14" t="s">
         <v>950</v>
       </c>
@@ -69708,7 +69708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A346" s="14" t="s">
         <v>951</v>
       </c>
@@ -69873,7 +69873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A347" s="5" t="s">
         <v>954</v>
       </c>
@@ -70038,7 +70038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A348" s="5" t="s">
         <v>957</v>
       </c>
@@ -70203,7 +70203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A349" s="14" t="s">
         <v>961</v>
       </c>
@@ -70368,7 +70368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A350" s="14" t="s">
         <v>964</v>
       </c>
@@ -70529,7 +70529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A351" s="14" t="s">
         <v>967</v>
       </c>
@@ -70692,7 +70692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A352" s="14" t="s">
         <v>969</v>
       </c>
@@ -70853,7 +70853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A353" s="5" t="s">
         <v>971</v>
       </c>
@@ -71016,7 +71016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A354" s="14" t="s">
         <v>974</v>
       </c>
@@ -71177,7 +71177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A355" s="14" t="s">
         <v>976</v>
       </c>
@@ -71340,7 +71340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A356" s="14" t="s">
         <v>978</v>
       </c>
@@ -71503,7 +71503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A357" s="5" t="s">
         <v>981</v>
       </c>
@@ -71664,7 +71664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A358" s="5" t="s">
         <v>983</v>
       </c>
@@ -71829,7 +71829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A359" s="5" t="s">
         <v>986</v>
       </c>
@@ -71998,7 +71998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A360" s="14" t="s">
         <v>989</v>
       </c>
@@ -72167,7 +72167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A361" s="14" t="s">
         <v>991</v>
       </c>
@@ -72334,7 +72334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A362" s="14" t="s">
         <v>995</v>
       </c>
@@ -72499,7 +72499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A363" s="5" t="s">
         <v>997</v>
       </c>
@@ -72664,7 +72664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A364" s="14" t="s">
         <v>1000</v>
       </c>
@@ -72829,7 +72829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A365" s="14" t="s">
         <v>1002</v>
       </c>
@@ -72992,7 +72992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:80" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A366" s="5" t="s">
         <v>1003</v>
       </c>
@@ -73155,7 +73155,7 @@
       </c>
       <c r="CB366" s="24"/>
     </row>
-    <row r="367" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A367" s="14" t="s">
         <v>1007</v>
       </c>
@@ -73318,7 +73318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:80" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:80" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A368" s="14" t="s">
         <v>1010</v>
       </c>
@@ -73475,7 +73475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A369" s="14" t="s">
         <v>1014</v>
       </c>
@@ -73632,7 +73632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A370" s="14" t="s">
         <v>1016</v>
       </c>
@@ -73785,7 +73785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A371" s="14" t="s">
         <v>1019</v>
       </c>
@@ -73938,7 +73938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:77" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:77" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A372" s="14" t="s">
         <v>1023</v>
       </c>
@@ -74091,7 +74091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:77" s="19" customFormat="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:77" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A373" s="9" t="s">
         <v>1026</v>
       </c>
@@ -74254,7 +74254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:77" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:77" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A374" s="5" t="s">
         <v>1029</v>
       </c>
@@ -74417,7 +74417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A375" s="5" t="s">
         <v>1032</v>
       </c>
@@ -74580,7 +74580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A376" s="14" t="s">
         <v>1034</v>
       </c>
@@ -74742,7 +74742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A377" s="5" t="s">
         <v>1036</v>
       </c>
@@ -74905,7 +74905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A378" s="14" t="s">
         <v>1037</v>
       </c>
@@ -75067,7 +75067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A379" s="14" t="s">
         <v>1039</v>
       </c>
@@ -75229,7 +75229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A380" s="14" t="s">
         <v>1042</v>
       </c>
@@ -75387,7 +75387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A381" s="14" t="s">
         <v>1044</v>
       </c>
@@ -75545,7 +75545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A382" s="14" t="s">
         <v>1047</v>
       </c>
@@ -75701,7 +75701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:77" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:77" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A383" s="14" t="s">
         <v>1050</v>
       </c>
@@ -75857,7 +75857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:77" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:77" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A384" s="5" t="s">
         <v>1053</v>
       </c>
@@ -76020,7 +76020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A385" s="5" t="s">
         <v>1054</v>
       </c>
@@ -76183,7 +76183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="386" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A386" s="14" t="s">
         <v>1056</v>
       </c>
@@ -76345,7 +76345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="387" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A387" s="5" t="s">
         <v>1058</v>
       </c>
@@ -76508,7 +76508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A388" s="14" t="s">
         <v>1060</v>
       </c>
@@ -76671,7 +76671,7 @@
       </c>
       <c r="CB388" s="24"/>
     </row>
-    <row r="389" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A389" s="14" t="s">
         <v>1062</v>
       </c>
@@ -76833,7 +76833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="390" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A390" s="14" t="s">
         <v>1064</v>
       </c>
@@ -76991,7 +76991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="391" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A391" s="14" t="s">
         <v>1066</v>
       </c>
@@ -77149,7 +77149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="392" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A392" s="14" t="s">
         <v>1069</v>
       </c>
@@ -77307,7 +77307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A393" s="14" t="s">
         <v>1071</v>
       </c>
@@ -77463,7 +77463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="394" spans="1:80" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A394" s="5" t="s">
         <v>1073</v>
       </c>
@@ -77623,7 +77623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A395" s="14" t="s">
         <v>1076</v>
       </c>
@@ -77784,7 +77784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="396" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A396" s="14" t="s">
         <v>1079</v>
       </c>
@@ -77941,7 +77941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="397" spans="1:80" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:80" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A397" s="5" t="s">
         <v>1082</v>
       </c>
@@ -78093,7 +78093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A398" s="14" t="s">
         <v>1084</v>
       </c>
@@ -78246,7 +78246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="399" spans="1:80" s="28" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:80" s="28" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A399" s="6" t="s">
         <v>1086</v>
       </c>
@@ -78407,7 +78407,7 @@
       </c>
       <c r="CB399" s="29"/>
     </row>
-    <row r="400" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A400" s="14" t="s">
         <v>1089</v>
       </c>
@@ -78568,7 +78568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="401" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A401" s="14" t="s">
         <v>1092</v>
       </c>
@@ -78729,7 +78729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="402" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A402" s="14" t="s">
         <v>1095</v>
       </c>
@@ -78888,7 +78888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="403" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A403" s="14" t="s">
         <v>1099</v>
       </c>
@@ -79047,7 +79047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="404" spans="1:80" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:80" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A404" s="14" t="s">
         <v>1102</v>
       </c>

</xml_diff>